<commit_message>
chore: adicionando gif de interface
</commit_message>
<xml_diff>
--- a/data/PROCESSOS.xlsx
+++ b/data/PROCESSOS.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuário\OneDrive\Área de Trabalho\ADVBOX PLANILHAS\Advbox Planilhas PADRÃO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maquina\Documents\projects\adv-box-teste-pratico\advbox-teste-pratico\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74622C21-A581-4D37-B1D5-FAE2197EEA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6555"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Página1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>NOME DO CLIENTE</t>
   </si>
@@ -82,33 +83,12 @@
   </si>
   <si>
     <t>ANOTAÇÕES GERAIS</t>
-  </si>
-  <si>
-    <t>Campo livre</t>
-  </si>
-  <si>
-    <t>0000000-00.0000.0.00.0000</t>
-  </si>
-  <si>
-    <t>Sigla do tribunal</t>
-  </si>
-  <si>
-    <t>dd/mm/aaaa</t>
-  </si>
-  <si>
-    <t>Precisa estar cadastrado como usuário ou ficar em branco</t>
-  </si>
-  <si>
-    <t>*obrigatório</t>
-  </si>
-  <si>
-    <t>Atendimento, Judicial, Administrativo, Arquivamento, Recursal, Execução/cobrança, Consultoria, RH/Financeiro, Marketing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -159,12 +139,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -380,19 +358,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,112 +434,62 @@
       <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="3">
-        <v>210.05</v>
-      </c>
-      <c r="M2" s="3">
-        <v>210.05</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>21</v>
-      </c>
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
-      <c r="Y3" s="5"/>
-      <c r="Z3" s="5"/>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>